<commit_message>
percentage.py and refine lots codes
</commit_message>
<xml_diff>
--- a/excel/AllRestInfo.xlsx
+++ b/excel/AllRestInfo.xlsx
@@ -1,15 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26812"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Workspace/yelp-line/excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="AllRest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -151,8 +161,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +199,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -235,12 +250,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -267,14 +282,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -301,6 +317,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,14 +493,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -500,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -517,10 +543,10 @@
         <v>16.0741316744427</v>
       </c>
       <c r="F3">
-        <v>3.30673665791776</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>3.3067366579177602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -537,10 +563,10 @@
         <v>10.8023394131642</v>
       </c>
       <c r="F4">
-        <v>3.65977634700102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>3.6597763470010198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -554,13 +580,13 @@
         <v>40</v>
       </c>
       <c r="E5">
-        <v>17.1363173957274</v>
+        <v>17.136317395727399</v>
       </c>
       <c r="F5">
-        <v>3.17513215352792</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>3.1751321535279202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -574,13 +600,13 @@
         <v>355</v>
       </c>
       <c r="E6">
-        <v>13.4979068550497</v>
+        <v>13.497906855049701</v>
       </c>
       <c r="F6">
         <v>3.60198720877113</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -600,7 +626,7 @@
         <v>3.99490740740741</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -620,7 +646,7 @@
         <v>3.48648648648649</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -637,10 +663,10 @@
         <v>15.5724519700423</v>
       </c>
       <c r="F9">
-        <v>3.59985593372952</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>3.5998559337295202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -654,13 +680,13 @@
         <v>109</v>
       </c>
       <c r="E10">
-        <v>13.6533599467731</v>
+        <v>13.653359946773101</v>
       </c>
       <c r="F10">
-        <v>4.02632348639953</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>4.0263234863995301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -674,13 +700,13 @@
         <v>106</v>
       </c>
       <c r="E11">
-        <v>20.0829659318637</v>
+        <v>20.082965931863701</v>
       </c>
       <c r="F11">
-        <v>3.30773249738767</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>3.3077324973876698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -694,13 +720,13 @@
         <v>182</v>
       </c>
       <c r="E12">
-        <v>22.4292216659081</v>
+        <v>22.429221665908099</v>
       </c>
       <c r="F12">
-        <v>4.14437459354</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>4.1443745935400003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -714,13 +740,13 @@
         <v>257</v>
       </c>
       <c r="E13">
-        <v>15.4381399317406</v>
+        <v>15.438139931740601</v>
       </c>
       <c r="F13">
-        <v>3.92279482725343</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>3.9227948272534299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -734,13 +760,13 @@
         <v>25</v>
       </c>
       <c r="E14">
-        <v>13.2058686539357</v>
+        <v>13.205868653935701</v>
       </c>
       <c r="F14">
         <v>3.26708074534162</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -757,10 +783,10 @@
         <v>7.66222222222222</v>
       </c>
       <c r="F15">
-        <v>3.71398305084746</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>3.7139830508474598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -774,13 +800,13 @@
         <v>161</v>
       </c>
       <c r="E16">
-        <v>10.3476360746921</v>
+        <v>10.347636074692099</v>
       </c>
       <c r="F16">
-        <v>3.51310043668122</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>3.5131004366812202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -794,13 +820,13 @@
         <v>66</v>
       </c>
       <c r="E17">
-        <v>12.7128129602356</v>
+        <v>12.712812960235601</v>
       </c>
       <c r="F17">
-        <v>3.65408805031447</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>3.6540880503144701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -814,13 +840,13 @@
         <v>31</v>
       </c>
       <c r="E18">
-        <v>11.7733031674208</v>
+        <v>11.773303167420799</v>
       </c>
       <c r="F18">
-        <v>3.31057563587684</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>3.3105756358768401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -834,13 +860,13 @@
         <v>10</v>
       </c>
       <c r="E19">
-        <v>12.8033492822967</v>
+        <v>12.803349282296701</v>
       </c>
       <c r="F19">
-        <v>5.09475195405966</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>5.0947519540596602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -854,13 +880,13 @@
         <v>200</v>
       </c>
       <c r="E20">
-        <v>11.6988764044944</v>
+        <v>11.698876404494399</v>
       </c>
       <c r="F20">
-        <v>3.61250592136428</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>3.6125059213642801</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -874,13 +900,13 @@
         <v>18</v>
       </c>
       <c r="E21">
-        <v>15.5924617196702</v>
+        <v>15.592461719670199</v>
       </c>
       <c r="F21">
-        <v>3.17086834733894</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>3.1708683473389399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -894,10 +920,10 @@
         <v>202</v>
       </c>
       <c r="E22">
-        <v>16.6761963952766</v>
+        <v>16.676196395276602</v>
       </c>
       <c r="F22">
-        <v>3.93090356871678</v>
+        <v>3.9309035687167801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>